<commit_message>
read value from excel
</commit_message>
<xml_diff>
--- a/data/G6_burning_time.xlsx
+++ b/data/G6_burning_time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JenRen\Documents\NCKU\IIM專題\GA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\Desktop\專題\GA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE38DEF2-3601-4CBE-A992-2AC636A9C359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC02433-2FDA-47C5-BBE8-585874CAAC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6888" yWindow="4440" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>i</t>
   </si>
   <si>
     <t>burning time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quantity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -356,68 +360,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>